<commit_message>
Add year filtering and refresh dataset labels
</commit_message>
<xml_diff>
--- a/backend/data/atlas/processed/contract_static/contract_state.xlsx
+++ b/backend/data/atlas/processed/contract_static/contract_state.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
   <si>
     <t>state</t>
   </si>
@@ -40,6 +40,18 @@
     <t>residents</t>
   </si>
   <si>
+    <t>fed_act_obl_per_1000</t>
+  </si>
+  <si>
+    <t>fed_act_obl_indirect_per_1000</t>
+  </si>
+  <si>
+    <t>subaward_amount_net_inflow_per_1000</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
     <t>alabama</t>
   </si>
   <si>
@@ -191,6 +203,9 @@
   </si>
   <si>
     <t>wyoming</t>
+  </si>
+  <si>
+    <t>Ave 2020-2024</t>
   </si>
 </sst>
 </file>
@@ -548,13 +563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,10 +594,22 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>15290765518.88834</v>
@@ -605,10 +632,22 @@
       <c r="H2">
         <v>15045</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>3025326</v>
+      </c>
+      <c r="J2">
+        <v>3043555</v>
+      </c>
+      <c r="K2">
+        <v>18228</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>6361752035.318401</v>
@@ -631,10 +670,22 @@
       <c r="H3">
         <v>5676</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>8667579</v>
+      </c>
+      <c r="J3">
+        <v>8401120</v>
+      </c>
+      <c r="K3">
+        <v>-266459</v>
+      </c>
+      <c r="L3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>23108212975.77254</v>
@@ -657,10 +708,22 @@
       <c r="H4">
         <v>23134</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>3179369</v>
+      </c>
+      <c r="J4">
+        <v>2982672</v>
+      </c>
+      <c r="K4">
+        <v>-196697</v>
+      </c>
+      <c r="L4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>753682656.911257</v>
@@ -683,10 +746,22 @@
       <c r="H5">
         <v>9722</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>248522</v>
+      </c>
+      <c r="J5">
+        <v>444627</v>
+      </c>
+      <c r="K5">
+        <v>196105</v>
+      </c>
+      <c r="L5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>60616129740.36436</v>
@@ -709,10 +784,22 @@
       <c r="H6">
         <v>79947</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>1544643</v>
+      </c>
+      <c r="J6">
+        <v>1679842</v>
+      </c>
+      <c r="K6">
+        <v>135198</v>
+      </c>
+      <c r="L6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>16469840645.00432</v>
@@ -735,10 +822,22 @@
       <c r="H7">
         <v>25239</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>2834362</v>
+      </c>
+      <c r="J7">
+        <v>2819877</v>
+      </c>
+      <c r="K7">
+        <v>-14485</v>
+      </c>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>22479859807.58086</v>
@@ -761,10 +860,22 @@
       <c r="H8">
         <v>6188</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>6247272</v>
+      </c>
+      <c r="J8">
+        <v>6427607</v>
+      </c>
+      <c r="K8">
+        <v>180335</v>
+      </c>
+      <c r="L8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>649243280.5445197</v>
@@ -787,10 +898,22 @@
       <c r="H9">
         <v>2749</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>645453</v>
+      </c>
+      <c r="J9">
+        <v>732677</v>
+      </c>
+      <c r="K9">
+        <v>87223</v>
+      </c>
+      <c r="L9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>9740520770.388897</v>
@@ -813,10 +936,22 @@
       <c r="H10">
         <v>25897</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>14493118</v>
+      </c>
+      <c r="J10">
+        <v>14664071</v>
+      </c>
+      <c r="K10">
+        <v>170952</v>
+      </c>
+      <c r="L10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>26102468437.80782</v>
@@ -839,10 +974,22 @@
       <c r="H11">
         <v>53303</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <v>1190323</v>
+      </c>
+      <c r="J11">
+        <v>1242541</v>
+      </c>
+      <c r="K11">
+        <v>52217</v>
+      </c>
+      <c r="L11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>8575900144.309906</v>
@@ -865,10 +1012,22 @@
       <c r="H12">
         <v>40990</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>792407</v>
+      </c>
+      <c r="J12">
+        <v>807340</v>
+      </c>
+      <c r="K12">
+        <v>14933</v>
+      </c>
+      <c r="L12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>2655295721.50517</v>
@@ -891,10 +1050,22 @@
       <c r="H13">
         <v>4815</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>1836767</v>
+      </c>
+      <c r="J13">
+        <v>1840403</v>
+      </c>
+      <c r="K13">
+        <v>3635</v>
+      </c>
+      <c r="L13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>3215552543.974854</v>
@@ -917,10 +1088,22 @@
       <c r="H14">
         <v>7465</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>1698388</v>
+      </c>
+      <c r="J14">
+        <v>1805608</v>
+      </c>
+      <c r="K14">
+        <v>107220</v>
+      </c>
+      <c r="L14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>14444692565.08573</v>
@@ -943,10 +1126,22 @@
       <c r="H15">
         <v>29556</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>1138035</v>
+      </c>
+      <c r="J15">
+        <v>1178882</v>
+      </c>
+      <c r="K15">
+        <v>40847</v>
+      </c>
+      <c r="L15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>5667464410.958149</v>
@@ -969,10 +1164,22 @@
       <c r="H16">
         <v>13196</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>832012</v>
+      </c>
+      <c r="J16">
+        <v>874012</v>
+      </c>
+      <c r="K16">
+        <v>42000</v>
+      </c>
+      <c r="L16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>2836675359.191178</v>
@@ -995,10 +1202,22 @@
       <c r="H17">
         <v>7648</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>887588</v>
+      </c>
+      <c r="J17">
+        <v>1072928</v>
+      </c>
+      <c r="K17">
+        <v>185340</v>
+      </c>
+      <c r="L17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>3681854677.085525</v>
@@ -1021,10 +1240,22 @@
       <c r="H18">
         <v>11729</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>1253367</v>
+      </c>
+      <c r="J18">
+        <v>1369272</v>
+      </c>
+      <c r="K18">
+        <v>115904</v>
+      </c>
+      <c r="L18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>11011075993.82397</v>
@@ -1047,10 +1278,22 @@
       <c r="H19">
         <v>11591</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>2441087</v>
+      </c>
+      <c r="J19">
+        <v>2403590</v>
+      </c>
+      <c r="K19">
+        <v>-37496</v>
+      </c>
+      <c r="L19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>3366302229.753199</v>
@@ -1073,10 +1316,22 @@
       <c r="H20">
         <v>12262</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>728475</v>
+      </c>
+      <c r="J20">
+        <v>742811</v>
+      </c>
+      <c r="K20">
+        <v>14335</v>
+      </c>
+      <c r="L20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <v>2519203178.773753</v>
@@ -1099,10 +1354,22 @@
       <c r="H21">
         <v>3687</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <v>1828955</v>
+      </c>
+      <c r="J21">
+        <v>1845519</v>
+      </c>
+      <c r="K21">
+        <v>16564</v>
+      </c>
+      <c r="L21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>50136976847.30976</v>
@@ -1125,10 +1392,22 @@
       <c r="H22">
         <v>121760</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <v>8124956</v>
+      </c>
+      <c r="J22">
+        <v>8064412</v>
+      </c>
+      <c r="K22">
+        <v>-60543</v>
+      </c>
+      <c r="L22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>22043329364.82252</v>
@@ -1151,10 +1430,22 @@
       <c r="H23">
         <v>17092</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <v>3152471</v>
+      </c>
+      <c r="J23">
+        <v>3246163</v>
+      </c>
+      <c r="K23">
+        <v>93691</v>
+      </c>
+      <c r="L23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>8589295196.162393</v>
@@ -1177,10 +1468,22 @@
       <c r="H24">
         <v>16771</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <v>854520</v>
+      </c>
+      <c r="J24">
+        <v>866437</v>
+      </c>
+      <c r="K24">
+        <v>11916</v>
+      </c>
+      <c r="L24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>3875441419.173976</v>
@@ -1203,10 +1506,22 @@
       <c r="H25">
         <v>14425</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <v>678269</v>
+      </c>
+      <c r="J25">
+        <v>739584</v>
+      </c>
+      <c r="K25">
+        <v>61314</v>
+      </c>
+      <c r="L25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>5810781484.178046</v>
@@ -1229,10 +1544,22 @@
       <c r="H26">
         <v>9723</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <v>1968796</v>
+      </c>
+      <c r="J26">
+        <v>1797518</v>
+      </c>
+      <c r="K26">
+        <v>-171278</v>
+      </c>
+      <c r="L26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>15417057490.6471</v>
@@ -1255,10 +1582,22 @@
       <c r="H27">
         <v>23721</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <v>2499449</v>
+      </c>
+      <c r="J27">
+        <v>2128572</v>
+      </c>
+      <c r="K27">
+        <v>-370877</v>
+      </c>
+      <c r="L27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>1146393507.955658</v>
@@ -1281,10 +1620,22 @@
       <c r="H28">
         <v>8039</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <v>1037392</v>
+      </c>
+      <c r="J28">
+        <v>1087843</v>
+      </c>
+      <c r="K28">
+        <v>50450</v>
+      </c>
+      <c r="L28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <v>1601999505.895856</v>
@@ -1307,10 +1658,22 @@
       <c r="H29">
         <v>5513</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <v>814882</v>
+      </c>
+      <c r="J29">
+        <v>860364</v>
+      </c>
+      <c r="K29">
+        <v>45481</v>
+      </c>
+      <c r="L29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>2790861108.12918</v>
@@ -1333,10 +1696,22 @@
       <c r="H30">
         <v>9749</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <v>888526</v>
+      </c>
+      <c r="J30">
+        <v>888709</v>
+      </c>
+      <c r="K30">
+        <v>183</v>
+      </c>
+      <c r="L30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B31">
         <v>2349860070.193745</v>
@@ -1359,10 +1734,22 @@
       <c r="H31">
         <v>4776</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31">
+        <v>1693185</v>
+      </c>
+      <c r="J31">
+        <v>2569270</v>
+      </c>
+      <c r="K31">
+        <v>876085</v>
+      </c>
+      <c r="L31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>12175001285.5153</v>
@@ -1385,10 +1772,22 @@
       <c r="H32">
         <v>15836</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <v>1313799</v>
+      </c>
+      <c r="J32">
+        <v>1333757</v>
+      </c>
+      <c r="K32">
+        <v>19957</v>
+      </c>
+      <c r="L32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B33">
         <v>6673125437.065495</v>
@@ -1411,10 +1810,22 @@
       <c r="H33">
         <v>14085</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33">
+        <v>3155488</v>
+      </c>
+      <c r="J33">
+        <v>3783832</v>
+      </c>
+      <c r="K33">
+        <v>628343</v>
+      </c>
+      <c r="L33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <v>24084637164.50908</v>
@@ -1437,10 +1848,22 @@
       <c r="H34">
         <v>38140</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34">
+        <v>1211969</v>
+      </c>
+      <c r="J34">
+        <v>1263702</v>
+      </c>
+      <c r="K34">
+        <v>51733</v>
+      </c>
+      <c r="L34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <v>6577778008.329524</v>
@@ -1463,10 +1886,22 @@
       <c r="H35">
         <v>24918</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35">
+        <v>621463</v>
+      </c>
+      <c r="J35">
+        <v>672893</v>
+      </c>
+      <c r="K35">
+        <v>51430</v>
+      </c>
+      <c r="L35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B36">
         <v>1042798655.657681</v>
@@ -1489,10 +1924,22 @@
       <c r="H36">
         <v>3075</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36">
+        <v>1338017</v>
+      </c>
+      <c r="J36">
+        <v>1370915</v>
+      </c>
+      <c r="K36">
+        <v>32898</v>
+      </c>
+      <c r="L36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B37">
         <v>14402172495.54946</v>
@@ -1515,10 +1962,22 @@
       <c r="H37">
         <v>26403</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37">
+        <v>1222590</v>
+      </c>
+      <c r="J37">
+        <v>940405</v>
+      </c>
+      <c r="K37">
+        <v>-282185</v>
+      </c>
+      <c r="L37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B38">
         <v>5889963223.027794</v>
@@ -1541,10 +2000,22 @@
       <c r="H38">
         <v>14784</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38">
+        <v>1474237</v>
+      </c>
+      <c r="J38">
+        <v>1459953</v>
+      </c>
+      <c r="K38">
+        <v>-14283</v>
+      </c>
+      <c r="L38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B39">
         <v>2395996483.94145</v>
@@ -1567,10 +2038,22 @@
       <c r="H39">
         <v>15219</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39">
+        <v>565264</v>
+      </c>
+      <c r="J39">
+        <v>626282</v>
+      </c>
+      <c r="K39">
+        <v>61017</v>
+      </c>
+      <c r="L39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B40">
         <v>18453426048.06388</v>
@@ -1593,10 +2076,22 @@
       <c r="H40">
         <v>37267</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40">
+        <v>1420967</v>
+      </c>
+      <c r="J40">
+        <v>1407597</v>
+      </c>
+      <c r="K40">
+        <v>-13370</v>
+      </c>
+      <c r="L40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>700386417.8387752</v>
@@ -1619,10 +2114,22 @@
       <c r="H41">
         <v>2772</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41">
+        <v>639405</v>
+      </c>
+      <c r="J41">
+        <v>652316</v>
+      </c>
+      <c r="K41">
+        <v>12910</v>
+      </c>
+      <c r="L41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B42">
         <v>10759584745.25349</v>
@@ -1645,10 +2152,22 @@
       <c r="H42">
         <v>12495</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42">
+        <v>2064080</v>
+      </c>
+      <c r="J42">
+        <v>2092141</v>
+      </c>
+      <c r="K42">
+        <v>28061</v>
+      </c>
+      <c r="L42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B43">
         <v>594454499.2862437</v>
@@ -1671,10 +2190,22 @@
       <c r="H43">
         <v>6236</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43">
+        <v>661097</v>
+      </c>
+      <c r="J43">
+        <v>760427</v>
+      </c>
+      <c r="K43">
+        <v>99330</v>
+      </c>
+      <c r="L43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B44">
         <v>10707152897.50643</v>
@@ -1697,10 +2228,22 @@
       <c r="H44">
         <v>19851</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44">
+        <v>1532640</v>
+      </c>
+      <c r="J44">
+        <v>1581062</v>
+      </c>
+      <c r="K44">
+        <v>48421</v>
+      </c>
+      <c r="L44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B45">
         <v>68486281570.69197</v>
@@ -1723,10 +2266,22 @@
       <c r="H45">
         <v>74057</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45">
+        <v>2310576</v>
+      </c>
+      <c r="J45">
+        <v>2068265</v>
+      </c>
+      <c r="K45">
+        <v>-242310</v>
+      </c>
+      <c r="L45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B46">
         <v>5055821602.419008</v>
@@ -1749,10 +2304,22 @@
       <c r="H46">
         <v>14936</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46">
+        <v>1517723</v>
+      </c>
+      <c r="J46">
+        <v>1841245</v>
+      </c>
+      <c r="K46">
+        <v>323521</v>
+      </c>
+      <c r="L46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B47">
         <v>813452578.7350634</v>
@@ -1775,10 +2342,22 @@
       <c r="H47">
         <v>2195</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47">
+        <v>1260670</v>
+      </c>
+      <c r="J47">
+        <v>1439670</v>
+      </c>
+      <c r="K47">
+        <v>178999</v>
+      </c>
+      <c r="L47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B48">
         <v>120881460956.2144</v>
@@ -1801,10 +2380,22 @@
       <c r="H48">
         <v>84966</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48">
+        <v>13962630</v>
+      </c>
+      <c r="J48">
+        <v>13604910</v>
+      </c>
+      <c r="K48">
+        <v>-357720</v>
+      </c>
+      <c r="L48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B49">
         <v>12243921251.26231</v>
@@ -1827,10 +2418,22 @@
       <c r="H49">
         <v>24233</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49">
+        <v>1581700</v>
+      </c>
+      <c r="J49">
+        <v>1584894</v>
+      </c>
+      <c r="K49">
+        <v>3194</v>
+      </c>
+      <c r="L49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B50">
         <v>717838411.5197668</v>
@@ -1853,10 +2456,22 @@
       <c r="H50">
         <v>13044</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50">
+        <v>402271</v>
+      </c>
+      <c r="J50">
+        <v>669922</v>
+      </c>
+      <c r="K50">
+        <v>267650</v>
+      </c>
+      <c r="L50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B51">
         <v>10000603268.4411</v>
@@ -1879,10 +2494,22 @@
       <c r="H51">
         <v>14214</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51">
+        <v>1697312</v>
+      </c>
+      <c r="J51">
+        <v>1738660</v>
+      </c>
+      <c r="K51">
+        <v>41348</v>
+      </c>
+      <c r="L51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B52">
         <v>175582028.2093317</v>
@@ -1904,6 +2531,18 @@
       </c>
       <c r="H52">
         <v>4198</v>
+      </c>
+      <c r="I52">
+        <v>302852</v>
+      </c>
+      <c r="J52">
+        <v>458409</v>
+      </c>
+      <c r="K52">
+        <v>155556</v>
+      </c>
+      <c r="L52" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>